<commit_message>
Definicion de presentación y otros apartados
</commit_message>
<xml_diff>
--- a/Documents/Rubrica para el proyecto de desarrollo colaborativo de un videojuego.xlsx
+++ b/Documents/Rubrica para el proyecto de desarrollo colaborativo de un videojuego.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\javiw\Documents\Master Profe\Practicas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javi\Documents\Master_profe\Practicas\Proyecto_intermodular\EjemploProyectoIntermodularDAM\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B6F4EF8-5865-4379-B470-07A71E2D2A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD003A0-F9D0-4B5E-9F89-D6FB59DF3D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FA01E2A3-A73B-4543-8BD2-CDAF2F4BD470}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FA01E2A3-A73B-4543-8BD2-CDAF2F4BD470}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rubrica" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,27 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
-  <si>
-    <t>Excelente</t>
-  </si>
-  <si>
-    <t>Adecuado</t>
-  </si>
-  <si>
-    <t>Básico</t>
-  </si>
-  <si>
-    <t>Insuficiente</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Uso incorrecto o inexistente del control de versiones.</t>
-  </si>
-  <si>
-    <t>Commits escasos o poco descriptivos. Escaso uso de ramas.</t>
-  </si>
-  <si>
-    <t>Uso básico de ramas y commits, con algunos problemas de organización.</t>
   </si>
   <si>
     <t>Uso correcto de ramas, commits frecuentes y descriptivos, validación entre compañeros y merges bien gestionados.</t>
@@ -97,61 +79,19 @@
     <t>No hay evidencia de planificación ni organización del trabajo.</t>
   </si>
   <si>
-    <t>Uso puntual de Trello o documentación mínima del proceso.</t>
-  </si>
-  <si>
-    <t>Trello utilizado de forma funcional, aunque con seguimiento irregular.</t>
-  </si>
-  <si>
-    <t>Uso continuo y coherente de Trello. Tareas bien definidas, asignadas y documentadas. Diario de desarrollo completo.</t>
-  </si>
-  <si>
     <t>No existe relación reconocible con los ODS.</t>
   </si>
   <si>
-    <t>Referencias poco claras o forzadas a los ODS.</t>
-  </si>
-  <si>
     <t>Los microjuegos integran de forma clara y coherente uno o varios ODS, reforzando el mensaje educativo.</t>
   </si>
   <si>
-    <t>Relación con algún ODS presente, aunque superficial en algunos microjuegos.</t>
-  </si>
-  <si>
-    <t>Microjuegos incompletos, repetitivos o inexistentes.</t>
-  </si>
-  <si>
-    <t>Se implementan los 12 microjuegos. Diversidad de diseños, objetivos y mecánicas, tiempo límite, interacción correcta y escalado de dificultad a partir de 10 y 20 puntos.</t>
-  </si>
-  <si>
-    <t>Algunos presentan mecánicas simples o repetitivas y dificultad mal diferenciada.</t>
-  </si>
-  <si>
-    <t>Número reducido de microjuegos o mecánicas poco claras. La dificultad no varía.</t>
-  </si>
-  <si>
     <t>No existe una estructura clara de juego o el proyecto no es jugable.</t>
   </si>
   <si>
-    <t>El juego funciona parcialmente, con una estructura confusa o incompleta.</t>
-  </si>
-  <si>
     <t>Estructura general correcta, aunque con problemas menores de navegación o cohesión.</t>
   </si>
   <si>
     <t>Juego bien estructurado, menú principal funcional, flujo claro entre microjuegos, sistema de vidas y puntuación correctamente implementados.</t>
-  </si>
-  <si>
-    <t>Repositorio y Pages configurados con pequeños errores menores que no impiden el uso del proyecto.</t>
-  </si>
-  <si>
-    <t>Repositorio correctamente configurado, GitHub Pages operativo, proyecto accesible desde la URL indicada. Uso correcto de ramas y estructura clara del proyecto.</t>
-  </si>
-  <si>
-    <t>Repositorio mal configurado o no accesible desde GitHub Pages.</t>
-  </si>
-  <si>
-    <t>Configuración incompleta o con errores que requieren intervención del para acceder al proyecto.</t>
   </si>
   <si>
     <r>
@@ -221,12 +161,69 @@
     <t>Rubrica para el proyecto de desarrollo colaborativo de un videojuego
 web usando metodologías ágiles</t>
   </si>
+  <si>
+    <t>Básico 50%</t>
+  </si>
+  <si>
+    <t>Adecuado 75%</t>
+  </si>
+  <si>
+    <t>Excelente 100%</t>
+  </si>
+  <si>
+    <t>Repositorio correctamente configurado, GitHub Pages operativo, proyecto accesible desde los URL indicados.</t>
+  </si>
+  <si>
+    <t>Repositorio correctamente configurado y accesible. GitHub Pages sin configurar.</t>
+  </si>
+  <si>
+    <t>Repositorio ni GitHub Pages accesible desde los URL entregados.</t>
+  </si>
+  <si>
+    <t>Insuficiente 0%</t>
+  </si>
+  <si>
+    <t>Referencias poco claras o incompletas uno o varios ODS.</t>
+  </si>
+  <si>
+    <t>Relación con varios ODS presentes, aunque superficial en algunos microjuegos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commits poco descriptivos. Se ha abierto más de una rama y su uso ha sido coherente. No se ha validado entre compañeros. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uso de ramas y commits coherente y descirptivo. Se ha validado una o varias funcionalidades, pero presentan algunos problemas de organización. </t>
+  </si>
+  <si>
+    <t>Uso continuo y coherente de Trello. Tareas bien definidas, asignadas y documentadas. Memoria de proyecto completa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trello utilizado de forma funcional, aunque la memoria demuestra un seguimiento irregular. </t>
+  </si>
+  <si>
+    <t>Uso de Trello: se han creado, gestionado y movido varias tareas. La memoria es limitada o incompleta.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No cumple con el número mínimo de microjuegos o no están correctamente diseñados. </t>
+  </si>
+  <si>
+    <t>Se implementan más de 6 microjuegos. Diversidad de diseños, objetivos y mecánicas. La dificultad está correctamente diferenciada y escala a partir de 10 y 20 puntos.</t>
+  </si>
+  <si>
+    <t>Cumple con el número mínimo de microjuegos correctamente diferenciados e implementados. La dificultad está correctamente diferenciada y escala a partir de 10 y 20 puntos.</t>
+  </si>
+  <si>
+    <t>Cumple con el número mínimo de microjuegos correctamente diferenciados e implementados. La dificultad no varía.</t>
+  </si>
+  <si>
+    <t>El juego funciona parcialmente, la estructura es incompleta.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,10 +340,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -685,142 +682,140 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E1E00F3-7182-477D-82AD-17B1443A866E}">
   <dimension ref="B1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="58.796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="36.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.09765625" style="1" customWidth="1"/>
     <col min="6" max="6" width="54" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="1"/>
+    <col min="7" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="8"/>
+    <row r="1" spans="2:6" ht="57.75" customHeight="1">
+      <c r="B1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" ht="15.6">
       <c r="B2" s="3"/>
       <c r="C2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="57" customHeight="1">
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="66" customHeight="1">
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="66" customHeight="1">
+      <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="C5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="54.75" customHeight="1">
+      <c r="B6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="57.75" customHeight="1">
+      <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>0</v>
+      <c r="C7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="6" t="s">
+    <row r="8" spans="2:6" ht="63" customHeight="1">
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rubrica actualizada, cambios menores
</commit_message>
<xml_diff>
--- a/Documents/Rubrica para el proyecto de desarrollo colaborativo de un videojuego.xlsx
+++ b/Documents/Rubrica para el proyecto de desarrollo colaborativo de un videojuego.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javi\Documents\Master_profe\Practicas\Proyecto_intermodular\EjemploProyectoIntermodularDAM\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1375ECFC-D10D-4AC0-A4A5-600BAE887230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8669BA-EC6B-4835-85BE-3A5111ED4B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FA01E2A3-A73B-4543-8BD2-CDAF2F4BD470}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
   <si>
     <t>Uso incorrecto o inexistente del control de versiones.</t>
   </si>
@@ -170,13 +170,16 @@
   </si>
   <si>
     <t>/10</t>
+  </si>
+  <si>
+    <t>Se implementan más del numero mínimo de microjuegos. Diversidad de diseños, objetivos y mecánicas. La dificultad está correctamente diferenciada y escala a partir de 10 y 20 puntos.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +233,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -335,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -367,6 +378,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -388,7 +402,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -750,46 +764,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15"/>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="16"/>
+      <c r="B1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="16" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="16" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="16" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="17"/>
+      <c r="J2" s="18"/>
       <c r="K2" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
@@ -822,7 +836,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
@@ -855,7 +869,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
@@ -888,7 +902,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -921,7 +935,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
@@ -954,7 +968,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="4" t="s">
         <v>30</v>
       </c>
@@ -967,11 +981,11 @@
       <c r="E8" s="6">
         <v>3</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
       <c r="I8" s="6">
         <v>6</v>
       </c>
@@ -983,7 +997,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="4" t="s">
         <v>31</v>
       </c>
@@ -1060,7 +1074,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1081,46 +1095,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15"/>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="16"/>
+      <c r="B1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="16" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="16" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="16" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="17"/>
+      <c r="J2" s="18"/>
       <c r="K2" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
@@ -1155,14 +1169,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="6">
         <v>0</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="19" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="6">
@@ -1183,14 +1197,14 @@
         <v>2</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="K4" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1225,7 +1239,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -1260,7 +1274,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
@@ -1295,7 +1309,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="4" t="s">
         <v>30</v>
       </c>
@@ -1309,11 +1323,11 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
       <c r="I8" s="6">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -1326,7 +1340,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="4" t="s">
         <v>31</v>
       </c>
@@ -1361,7 +1375,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K10" s="18">
+      <c r="K10" s="11">
         <f>SUM(K3:K9)</f>
         <v>10</v>
       </c>

</xml_diff>